<commit_message>
CCES Data Updates Updates c
</commit_message>
<xml_diff>
--- a/DemographicData.xlsx
+++ b/DemographicData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40df6d813d81318a/Documents/Neighborhood Watch Gang/badlands/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Documents\Neighborhood Watch Gang\badlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{80716D18-584F-46E4-962E-8F0CE2E63899}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{42CDB842-BE58-4377-95CA-9201C6F89139}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{80716D18-584F-46E4-962E-8F0CE2E63899}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{159E1FA6-ED03-41C7-9428-E4813CDF8814}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7260" xr2:uid="{57C289DB-0CD0-4B19-86D2-C03D3ADBE228}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>College Educated Rate</t>
+  </si>
+  <si>
+    <t>% National Turnout VEP</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FED7CE8-2CF6-4D6E-99C7-BA564000482B}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M16:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +539,7 @@
     <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,8 +597,11 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2006</v>
       </c>
@@ -651,8 +657,11 @@
       <c r="S2" s="5">
         <v>0.26850000000000002</v>
       </c>
+      <c r="T2" s="5">
+        <v>0.40400000000000003</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2008</v>
       </c>
@@ -710,8 +719,11 @@
       <c r="S3" s="5">
         <v>0.27310000000000001</v>
       </c>
+      <c r="T3" s="5">
+        <v>0.61599999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2010</v>
       </c>
@@ -769,8 +781,11 @@
       <c r="S4" s="5">
         <v>0.2792</v>
       </c>
+      <c r="T4" s="5">
+        <v>0.41</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2012</v>
       </c>
@@ -826,8 +841,11 @@
       <c r="S5" s="5">
         <v>0.28010000000000002</v>
       </c>
+      <c r="T5" s="5">
+        <v>0.58599999999999997</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2014</v>
       </c>
@@ -885,8 +903,11 @@
       <c r="S6" s="5">
         <v>0.28000000000000003</v>
       </c>
+      <c r="T6" s="5">
+        <v>0.36699999999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2016</v>
       </c>
@@ -944,8 +965,11 @@
       <c r="S7" s="5">
         <v>0.29559999999999997</v>
       </c>
+      <c r="T7" s="5">
+        <v>0.60099999999999998</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2018</v>
       </c>
@@ -1000,6 +1024,9 @@
       <c r="R8" s="1"/>
       <c r="S8" s="5">
         <v>0.30170000000000002</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>